<commit_message>
[Anmol Singh]Class ExcelWriter-Finalizing Classes-1.3
</commit_message>
<xml_diff>
--- a/Output_vehicle_Rental_System.xlsx
+++ b/Output_vehicle_Rental_System.xlsx
@@ -176,7 +176,7 @@
     <t>Me_AnmolSingh</t>
   </si>
   <si>
-    <t>JcsQTVLGk/LPMTwaTiQHWTiu6bdLuwCSqGN/h1DFTB8=</t>
+    <t>VhlR0Ri54zs6IP8BvQnP71b9Ky4EihDCJzMRDoovolw=</t>
   </si>
   <si>
     <t>ghtutgd</t>
@@ -206,7 +206,7 @@
     <t>Me_AmanKaur</t>
   </si>
   <si>
-    <t>r4t4IhD/SPdh+DOe+tHS8HIZznwRmIWp9pNh/2kmlSU=</t>
+    <t>pLGOpqK95Hty6A/lvZ3Xrf/EBxNi8NttV9AfDZTne68=</t>
   </si>
   <si>
     <t>458954hgtfr</t>
@@ -233,7 +233,7 @@
     <t>Me_inshant</t>
   </si>
   <si>
-    <t>BBvEspyJJJZO8TrUa6nhm16n3yJ/BKy4RlChm1FKy/w=</t>
+    <t>aCNUls5CZkC52JM941K1fn2QOdAcu4VwhMxQXZCs/4c=</t>
   </si>
   <si>
     <t>inshant</t>
@@ -257,7 +257,7 @@
     <t>Me_Monica</t>
   </si>
   <si>
-    <t>eIO89WWcHYkLwJeYPZei3E+nDt3EkZXnmx3p9t+9zhg=</t>
+    <t>WM9Y4GJX0raTMidHg1bDWGcI8rIXU/mnq3pJzjoYriM=</t>
   </si>
   <si>
     <t>5485lkjhy</t>
@@ -284,7 +284,7 @@
     <t>Ikroop_Virk</t>
   </si>
   <si>
-    <t>flhHkRMaZfgdsYCCS8EKn68WVnE0KhOCyA1zrdsXwS4=</t>
+    <t>NWvnVJ9pVFxDe/nmpQtemG6fablaH1QsIkgySyfP2/U=</t>
   </si>
   <si>
     <t>virkikroop</t>
@@ -305,7 +305,7 @@
     <t>Me_kritima</t>
   </si>
   <si>
-    <t>EVTHLaF9WE6nmDvsA8r3OKaj0IQaGhs+qUOskok5Pgg=</t>
+    <t>R4A/r4DiSZYWaonQTnBevEzB2IU0HaotW8XsCGC7NDU=</t>
   </si>
   <si>
     <t>5475lkmnj</t>
@@ -320,7 +320,7 @@
     <t>Me_param</t>
   </si>
   <si>
-    <t>uW6XbuwfrUj9wp3srLaHk9XuhvVZPZpYhpBuBRZ4Jc0=</t>
+    <t>hEgnKXwYI2HgzuQzfWK3VMoOeE9BgwdZmWi7YFHiCIY=</t>
   </si>
   <si>
     <t>paramkaur</t>
@@ -344,7 +344,7 @@
     <t>KumarShanu</t>
   </si>
   <si>
-    <t>iaBhJMSecCe+JjS56wFNl3ZQenpgiAVm0jNGV9oa59A=</t>
+    <t>7rPiSdEWKPrjdb1Zmx9PAa0JKHKo9JFsx37i7xOyKOU=</t>
   </si>
   <si>
     <t>kjhujh</t>
@@ -371,7 +371,7 @@
     <t>Jordan_Micheal</t>
   </si>
   <si>
-    <t>gTX1phNuGoR79FAVEzXC/jP6yhjh8f3VFOpndA0x1dc=</t>
+    <t>G0V2Fl+CMpoaNeM0dsaoxFLNM9fETBGU8w7knxXb3Qc=</t>
   </si>
   <si>
     <t>dfgtre3</t>
@@ -398,7 +398,7 @@
     <t>michelle</t>
   </si>
   <si>
-    <t>I+YF8Dh42yiuSq9IwEqphtapsCvzHGN/Fb0UbLviOXE=</t>
+    <t>OJ12sRQDM2gVNBXlNpnFYirvbN9EmSJZKU/HCJVdFZM=</t>
   </si>
   <si>
     <t>1254gytr</t>
@@ -422,7 +422,7 @@
     <t>SherinG</t>
   </si>
   <si>
-    <t>w1juPlKPGCKreGww2XB/9xhxzvMpbbIsZRXxJThvD1Y=</t>
+    <t>TtwMDMCKghM5vseiz222PJdsApIBOCOaC7lmCuOODzs=</t>
   </si>
   <si>
     <t>524plo;</t>
@@ -446,7 +446,7 @@
     <t>JainSaab</t>
   </si>
   <si>
-    <t>jciJqYzFnNlVPuD+ywrnhy2mElwzG8FyXSDl1QX8I2k=</t>
+    <t>4lcjkKxAaqRynj7giHPPGfBMuO0ihCXLb1zW96eEO2Q=</t>
   </si>
   <si>
     <t>ppo;;lko</t>
@@ -464,7 +464,7 @@
     <t>6723367567</t>
   </si>
   <si>
-    <t>8qzg4vQrh5ljymMMRJ8GVKaectY8i9fsDF6pFAKLdnY=</t>
+    <t>9ZMkCSYWW7t2WHpuuSIFqCoseEf41vCXlpD674ghuwE=</t>
   </si>
   <si>
     <t>ghat</t>
@@ -491,7 +491,7 @@
     <t>gillingum@gillingum.com</t>
   </si>
   <si>
-    <t>rdOTCgyiJLZZZMBEmv/56JeEiFkOv9SOZKl5ZA4uZZo=</t>
+    <t>7QdQOQOIpA0xhhblt1UxDV2V7/qWLguKNtjGLKv5L8A=</t>
   </si>
   <si>
     <t>dhobi_ghat</t>
@@ -518,7 +518,7 @@
     <t>careem@me.com</t>
   </si>
   <si>
-    <t>7DhpOFpv/5i6q1Co2WFzA2B9StAJSj75CjxBaQTFUHs=</t>
+    <t>y2cIG2ykg4FMvTJPQnhXR8F4qc0K4XJaKNlRAc3yxwA=</t>
   </si>
   <si>
     <t>Gaziattack</t>
@@ -563,7 +563,7 @@
     <t>Mercedes</t>
   </si>
   <si>
-    <t>IP4</t>
+    <t>IP1</t>
   </si>
   <si>
     <t>Petrol</t>
@@ -584,6 +584,9 @@
     <t>Hyundai</t>
   </si>
   <si>
+    <t>IP3</t>
+  </si>
+  <si>
     <t>Electric</t>
   </si>
   <si>
@@ -611,33 +614,30 @@
     <t>BMW</t>
   </si>
   <si>
+    <t>1J4BA6H11AL289387</t>
+  </si>
+  <si>
+    <t>Bullet</t>
+  </si>
+  <si>
+    <t>Royal Enfield</t>
+  </si>
+  <si>
+    <t>5LMCJ1A97FUJ59251</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>BusCompany-A</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
     <t>IP8</t>
   </si>
   <si>
-    <t>1J4BA6H11AL289387</t>
-  </si>
-  <si>
-    <t>Bullet</t>
-  </si>
-  <si>
-    <t>Royal Enfield</t>
-  </si>
-  <si>
-    <t>5LMCJ1A97FUJ59251</t>
-  </si>
-  <si>
-    <t>Volvo</t>
-  </si>
-  <si>
-    <t>BusCompany-A</t>
-  </si>
-  <si>
-    <t>Micheal</t>
-  </si>
-  <si>
-    <t>IP2</t>
-  </si>
-  <si>
     <t>1G1ZT548X5F147693</t>
   </si>
   <si>
@@ -647,7 +647,7 @@
     <t>BusCompany-B</t>
   </si>
   <si>
-    <t>IP1</t>
+    <t>IP6</t>
   </si>
   <si>
     <t>DoubleDecker</t>
@@ -764,7 +764,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="20.828125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.8203125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="51.44140625" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="51.93359375" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="12.28125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="10.59375" customWidth="true" bestFit="true"/>
@@ -822,7 +822,7 @@
         <v>48</v>
       </c>
       <c r="E2" t="n" s="2">
-        <v>35749.69153668982</v>
+        <v>35749.70926364583</v>
       </c>
       <c r="F2" t="s">
         <v>49</v>
@@ -860,7 +860,7 @@
         <v>58</v>
       </c>
       <c r="E3" t="n" s="2">
-        <v>35637.69153668982</v>
+        <v>35637.70926364583</v>
       </c>
       <c r="F3" t="s">
         <v>59</v>
@@ -898,7 +898,7 @@
         <v>48</v>
       </c>
       <c r="E4" t="n" s="2">
-        <v>35445.69153668982</v>
+        <v>35445.70926364583</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
@@ -936,7 +936,7 @@
         <v>58</v>
       </c>
       <c r="E5" t="n" s="2">
-        <v>35602.69153668982</v>
+        <v>35602.70926364583</v>
       </c>
       <c r="F5" t="s">
         <v>76</v>
@@ -974,7 +974,7 @@
         <v>58</v>
       </c>
       <c r="E6" t="n" s="2">
-        <v>34912.69153668982</v>
+        <v>34912.70926364583</v>
       </c>
       <c r="F6" t="s">
         <v>85</v>
@@ -1012,7 +1012,7 @@
         <v>58</v>
       </c>
       <c r="E7" t="n" s="2">
-        <v>35567.69153668982</v>
+        <v>35567.70926364583</v>
       </c>
       <c r="F7" t="s">
         <v>92</v>
@@ -1050,7 +1050,7 @@
         <v>58</v>
       </c>
       <c r="E8" t="n" s="2">
-        <v>33783.69153668982</v>
+        <v>33783.70926364583</v>
       </c>
       <c r="F8" t="s">
         <v>92</v>
@@ -1096,7 +1096,7 @@
     <col min="7" max="7" width="5.77734375" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="21.96875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="15.25" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="49.41015625" customWidth="true" bestFit="true"/>
+    <col min="10" max="10" width="52.62890625" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="20.04296875" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="18.6328125" customWidth="true" bestFit="true"/>
@@ -1161,7 +1161,7 @@
         <v>48</v>
       </c>
       <c r="E2" t="n" s="3">
-        <v>35735.69153668982</v>
+        <v>35735.70926364583</v>
       </c>
       <c r="F2" t="s">
         <v>105</v>
@@ -1205,7 +1205,7 @@
         <v>48</v>
       </c>
       <c r="E3" t="n" s="3">
-        <v>28476.691536689814</v>
+        <v>28476.709263645833</v>
       </c>
       <c r="F3" t="s">
         <v>114</v>
@@ -1249,7 +1249,7 @@
         <v>58</v>
       </c>
       <c r="E4" t="n" s="3">
-        <v>36936.69153668982</v>
+        <v>36936.70926364583</v>
       </c>
       <c r="F4" t="s">
         <v>123</v>
@@ -1293,7 +1293,7 @@
         <v>58</v>
       </c>
       <c r="E5" t="n" s="3">
-        <v>31279.691536689814</v>
+        <v>31279.709263645833</v>
       </c>
       <c r="F5" t="s">
         <v>131</v>
@@ -1337,7 +1337,7 @@
         <v>48</v>
       </c>
       <c r="E6" t="n" s="3">
-        <v>23923.691536689814</v>
+        <v>23923.709263645833</v>
       </c>
       <c r="F6" t="s">
         <v>139</v>
@@ -1388,7 +1388,7 @@
     <col min="6" max="6" width="13.96875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="23.7265625" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.23828125" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="48.96875" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="51.75" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="22.3359375" customWidth="true" bestFit="true"/>
     <col min="11" max="11" width="18.09375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="17.89453125" customWidth="true" bestFit="true"/>
@@ -1454,7 +1454,7 @@
         <v>58</v>
       </c>
       <c r="E2" t="n" s="4">
-        <v>29842.691536689814</v>
+        <v>29842.709263645833</v>
       </c>
       <c r="F2" t="s">
         <v>147</v>
@@ -1495,7 +1495,7 @@
         <v>48</v>
       </c>
       <c r="E3" t="n" s="4">
-        <v>28251.691536689814</v>
+        <v>28251.709263645833</v>
       </c>
       <c r="F3" t="s">
         <v>155</v>
@@ -1536,7 +1536,7 @@
         <v>58</v>
       </c>
       <c r="E4" t="n" s="4">
-        <v>29677.691536689814</v>
+        <v>29677.709263645833</v>
       </c>
       <c r="F4" t="s">
         <v>164</v>
@@ -1580,7 +1580,7 @@
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.70703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.51953125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
@@ -1685,7 +1685,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1730,19 +1730,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="H4" t="n">
         <v>5.0</v>
       </c>
       <c r="I4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J4" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K4" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L4" t="n">
         <v>100.0</v>
@@ -1822,13 +1822,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B2" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1859,13 +1859,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C3" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="G3" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="H3" t="n">
         <v>2.0</v>
@@ -1950,7 +1950,7 @@
     <col min="2" max="2" width="23.8125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="25.03515625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="13.63671875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="8.51953125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="8.70703125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="11.921875" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="30.76171875" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="15.09375" customWidth="true" bestFit="true"/>
@@ -2064,7 +2064,7 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -2249,7 +2249,7 @@
         <v>12.0</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F4" t="s">
         <v>223</v>

</xml_diff>